<commit_message>
SSDQMvsISO21001 v1.0; wskaźniki v0.1
</commit_message>
<xml_diff>
--- a/pomocnicze/SSDQMvsISO21001.xlsx
+++ b/pomocnicze/SSDQMvsISO21001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPSZ\Desktop\STUDIA\doktorat_git\pomocnicze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EC8BEC-EB3F-496E-8736-DFA8089E04AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4782361F-7DB5-458D-9C8C-6B8CFB578FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="0" windowWidth="11460" windowHeight="13500" firstSheet="2" activeTab="3" xr2:uid="{9E83F4E7-F310-436B-A179-0F14A6088F0A}"/>
+    <workbookView xWindow="983" yWindow="-98" windowWidth="23115" windowHeight="13695" firstSheet="2" activeTab="3" xr2:uid="{9E83F4E7-F310-436B-A179-0F14A6088F0A}"/>
   </bookViews>
   <sheets>
     <sheet name="PivotSSDQM" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="344">
   <si>
     <t>SSDQM vs ISO 21001</t>
   </si>
@@ -1080,9 +1080,6 @@
     <t>ogólny</t>
   </si>
   <si>
-    <t>całość tego dotyczy, szczególnie 6.</t>
-  </si>
-  <si>
     <t>"9.6"</t>
   </si>
   <si>
@@ -1183,6 +1180,12 @@
   </si>
   <si>
     <t>"9.3, 9.8</t>
+  </si>
+  <si>
+    <t>całość pierwszej fazy tego dotyczy, szczególnie 6.</t>
+  </si>
+  <si>
+    <t>"9.7</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1357,7 +1360,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -3155,14 +3157,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB15455-543F-47AE-B779-63D63ACEA602}">
   <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="65.53125" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -3206,7 +3208,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="19" t="s">
+      <c r="A6" t="s">
         <v>115</v>
       </c>
       <c r="B6" t="s">
@@ -3215,18 +3217,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
@@ -3289,7 +3291,7 @@
         <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -3297,7 +3299,7 @@
         <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
@@ -3305,7 +3307,7 @@
         <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
@@ -3313,7 +3315,7 @@
         <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -3321,7 +3323,7 @@
         <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>308</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
@@ -3329,7 +3331,7 @@
         <v>197</v>
       </c>
       <c r="B22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
@@ -3425,7 +3427,7 @@
         <v>209</v>
       </c>
       <c r="B34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
@@ -3449,7 +3451,7 @@
         <v>212</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -3457,7 +3459,7 @@
         <v>213</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
@@ -3513,7 +3515,7 @@
         <v>216</v>
       </c>
       <c r="B45" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
@@ -3529,7 +3531,7 @@
         <v>218</v>
       </c>
       <c r="B47" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
@@ -3553,7 +3555,7 @@
         <v>221</v>
       </c>
       <c r="B50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
@@ -3561,7 +3563,7 @@
         <v>222</v>
       </c>
       <c r="B51" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
@@ -3609,7 +3611,7 @@
         <v>228</v>
       </c>
       <c r="B57" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
@@ -3697,7 +3699,7 @@
         <v>239</v>
       </c>
       <c r="B68" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
@@ -3705,7 +3707,7 @@
         <v>240</v>
       </c>
       <c r="B69" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
@@ -3745,7 +3747,7 @@
         <v>245</v>
       </c>
       <c r="B74" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
@@ -3833,7 +3835,7 @@
         <v>256</v>
       </c>
       <c r="B85" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
@@ -4009,7 +4011,7 @@
         <v>278</v>
       </c>
       <c r="B107" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
@@ -4017,20 +4019,23 @@
         <v>279</v>
       </c>
       <c r="B108" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109" s="10" t="s">
         <v>280</v>
       </c>
+      <c r="B109" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>281</v>
       </c>
       <c r="B110" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
@@ -4038,7 +4043,7 @@
         <v>282</v>
       </c>
       <c r="B111" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
@@ -4054,7 +4059,7 @@
         <v>284</v>
       </c>
       <c r="B113" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
@@ -4062,7 +4067,7 @@
         <v>285</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
@@ -4070,7 +4075,7 @@
         <v>286</v>
       </c>
       <c r="B115" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
@@ -4078,7 +4083,7 @@
         <v>287</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
@@ -4086,7 +4091,7 @@
         <v>288</v>
       </c>
       <c r="B117" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
@@ -4110,7 +4115,7 @@
         <v>291</v>
       </c>
       <c r="B120" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
@@ -4118,25 +4123,31 @@
         <v>292</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" s="10" t="s">
         <v>293</v>
       </c>
+      <c r="B122" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" s="10" t="s">
         <v>294</v>
       </c>
+      <c r="B123" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" s="10" t="s">
         <v>295</v>
       </c>
       <c r="B124" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
@@ -4144,7 +4155,7 @@
         <v>296</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
@@ -4157,20 +4168,23 @@
         <v>298</v>
       </c>
       <c r="B127" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" s="10" t="s">
         <v>299</v>
       </c>
+      <c r="B128" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" s="10" t="s">
         <v>300</v>
       </c>
       <c r="B129" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
@@ -4178,7 +4192,7 @@
         <v>301</v>
       </c>
       <c r="B130" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>